<commit_message>
FMT5  Trabajamos con Excel     * eliminarFilasRepetidasExcel.ahk (Eliminamos filas repetidas segun una serie de columnas) (es decir eliminamos si A1 = A2 y B1 = B2 aunque los otros datos sean distintos quedandonos con la fila primera que se encuantra )     * ordenarExcelPorColumna.ahk (Solucionar cuando las filas de la columna tenga datos iguales) (es decir si A1=A2 no funciona bien)     * ordenarExcelPorColumna.ahk (Valoramos que tipo de dato es y segun sea ordenamos Nota: Incluir ordenar fecha)     * ordenarExcelPorColumna.ahk (Ordenar Ascendente o Descendente)     - eliminamos ficheros prueba para ordenarlos     + añadimos cartetas de Test para las pruebas     * Test_FMT1     * Test_FMT3     * Test_FMT4     * Test_FMT2     * validacionDatos.ahk (Validamos email)     * leerExcel.ahk (Funcion que te saca un elemento en concreto del excel)
</commit_message>
<xml_diff>
--- a/Datos_Prueba/Resultados/Test_FMT4/Excel_Filas_Ordenadas_1_ASC.xlsx
+++ b/Datos_Prueba/Resultados/Test_FMT4/Excel_Filas_Ordenadas_1_ASC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egarciar\Documents\CAIXA\AutoHotKeyEGR\Datos_Prueba\Resultados\Test_FMT4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{23E1A8FC-E7AD-4C7D-9128-96109BED7D63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{403A458A-362F-4505-A070-205CAFBDF6BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24800" yWindow="740" windowWidth="17570" windowHeight="8220" xr2:uid="{94942F74-4F45-4288-983E-BEA3848DA749}"/>
+    <workbookView xWindow="24800" yWindow="740" windowWidth="17570" windowHeight="8220" xr2:uid="{FAF5E5CB-7F43-444B-97D1-A37A52F4BAE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -551,7 +551,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57D1ED07-07A1-4A0B-BC73-25A5BE7EFF9A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C15AA584-A918-4696-A15C-8C5BA89D1034}">
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
FMT6  Trabajamos con Excel     * ordenarExcelPorColumna.ahk (Solucionar cuando las filas de la columna tenga datos iguales) (es decir si A1=A2 no funciona bien)     + buscarDatoExcel.ahk (Busca un elemento en el Excel y saca un informe de las posiciones donde se encuetra)     + TEST_FMT6.ahk     + Test_FMT4_C.ahk (Pruebas de ordenacion con datos repetidos en columnas)
</commit_message>
<xml_diff>
--- a/Datos_Prueba/Resultados/Test_FMT4/Excel_Filas_Ordenadas_1_ASC.xlsx
+++ b/Datos_Prueba/Resultados/Test_FMT4/Excel_Filas_Ordenadas_1_ASC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egarciar\Documents\CAIXA\AutoHotKeyEGR\Datos_Prueba\Resultados\Test_FMT4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{403A458A-362F-4505-A070-205CAFBDF6BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{142AFA11-6F8E-43A7-8546-271CB86EADD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24800" yWindow="740" windowWidth="17570" windowHeight="8220" xr2:uid="{FAF5E5CB-7F43-444B-97D1-A37A52F4BAE3}"/>
+    <workbookView xWindow="24800" yWindow="740" windowWidth="17570" windowHeight="8220" xr2:uid="{1FF83A8B-E2F4-4088-B79B-33B98C3980DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -551,7 +551,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C15AA584-A918-4696-A15C-8C5BA89D1034}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9377978-CD19-4E15-A2D4-3E4320147908}">
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>